<commit_message>
added manual calc of word example
</commit_message>
<xml_diff>
--- a/docs/reports/220831/smk_data_table.xlsx
+++ b/docs/reports/220831/smk_data_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\samer\projects\fuzzy_sql\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\samer\projects\fuzzy_sql\docs\reports\220831\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
     <t>&lt;=50K</t>
   </si>
@@ -171,12 +171,54 @@
   <si>
     <t>Per query Hellinger distance</t>
   </si>
+  <si>
+    <t>work_class</t>
+  </si>
+  <si>
+    <t>AVG(hours_per_week)</t>
+  </si>
+  <si>
+    <t>COUNTS</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>Divorced</t>
+  </si>
+  <si>
+    <t>Self-emp</t>
+  </si>
+  <si>
+    <t>Married</t>
+  </si>
+  <si>
+    <t>Local-gov</t>
+  </si>
+  <si>
+    <t>Never-married</t>
+  </si>
+  <si>
+    <t>Nan</t>
+  </si>
+  <si>
+    <t>prob</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>hlngr dist</t>
+  </si>
+  <si>
+    <t>std</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,8 +370,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Century Schoolbook"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Century Schoolbook"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,8 +569,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -631,6 +691,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -676,12 +797,30 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1047,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J59" sqref="J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,6 +1535,309 @@
         <v>0.12688998957080647</v>
       </c>
     </row>
+    <row r="51" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K52" t="s">
+        <v>53</v>
+      </c>
+      <c r="L52" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="8">
+        <v>39</v>
+      </c>
+      <c r="D53" s="8">
+        <v>219</v>
+      </c>
+      <c r="E53">
+        <f>D53/SUM(D53:D56)</f>
+        <v>0.79061371841155237</v>
+      </c>
+      <c r="I53">
+        <f>C53-C63</f>
+        <v>4</v>
+      </c>
+      <c r="J53">
+        <f>(I53-K53)/L53</f>
+        <v>0.70194976485069993</v>
+      </c>
+      <c r="K53">
+        <f>AVERAGE(I53:I55)</f>
+        <v>-6.6666666666667609E-2</v>
+      </c>
+      <c r="L53">
+        <f>STDEV(I53:I55)</f>
+        <v>5.7933870346571315</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="8">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="D54" s="8">
+        <v>9</v>
+      </c>
+      <c r="E54">
+        <f>D54/SUM(D53:D56)</f>
+        <v>3.2490974729241874E-2</v>
+      </c>
+      <c r="I54">
+        <f t="shared" ref="I54:I57" si="0">C54-C64</f>
+        <v>-6.7000000000000028</v>
+      </c>
+      <c r="J54">
+        <f>(I54-K53)/L53</f>
+        <v>-1.1449836328302403</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="8">
+        <v>41</v>
+      </c>
+      <c r="D55" s="8">
+        <v>29</v>
+      </c>
+      <c r="E55">
+        <f>D55/SUM(D53:D56)</f>
+        <v>0.10469314079422383</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="J55">
+        <f>(I55-K53)/L53</f>
+        <v>0.44303386797954025</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C56" s="8">
+        <v>36</v>
+      </c>
+      <c r="D56" s="8">
+        <v>20</v>
+      </c>
+      <c r="E56">
+        <f>D56/SUM(D53:D56)</f>
+        <v>7.2202166064981949E-2</v>
+      </c>
+      <c r="I56" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <f>SUM(E53:E56)</f>
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <f>(SQRT(E53)-SQRT(E63))^2</f>
+        <v>3.3226898170085331E-3</v>
+      </c>
+      <c r="J59">
+        <f>SQRT(J53^2+J54^2+J55^2)/3</f>
+        <v>0.47140452079103173</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G60">
+        <f t="shared" ref="G60:G63" si="1">(SQRT(E54)-SQRT(E64))^2</f>
+        <v>5.4656270270463825E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>5.2198390461093516E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>7.2202166064981962E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C63" s="8">
+        <v>35</v>
+      </c>
+      <c r="D63" s="8">
+        <v>121</v>
+      </c>
+      <c r="E63">
+        <f>D63/(SUM(D63:D65)+D67)</f>
+        <v>0.69142857142857139</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>1.714285714285714E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="8">
+        <v>40</v>
+      </c>
+      <c r="D64" s="8">
+        <v>30</v>
+      </c>
+      <c r="E64">
+        <f>D64/(SUM(D63:D65)+D67)</f>
+        <v>0.17142857142857143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" s="8">
+        <v>38.5</v>
+      </c>
+      <c r="D65" s="8">
+        <v>21</v>
+      </c>
+      <c r="E65">
+        <f>D65/(SUM(D63:D65)+D67)</f>
+        <v>0.12</v>
+      </c>
+      <c r="G65">
+        <f>(1/SQRT(2))*(SUM(G59:G63))^1/2</f>
+        <v>5.227144298907449E-2</v>
+      </c>
+      <c r="H65" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" s="8">
+        <v>39</v>
+      </c>
+      <c r="D67" s="8">
+        <v>3</v>
+      </c>
+      <c r="E67">
+        <f>D67/(SUM(D63:D65)+D67)</f>
+        <v>1.7142857142857144E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <f>SUM(E63:E65)+E67</f>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added index option to db
</commit_message>
<xml_diff>
--- a/docs/reports/220831/smk_data_table.xlsx
+++ b/docs/reports/220831/smk_data_table.xlsx
@@ -1188,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>